<commit_message>
add vs code tips
</commit_message>
<xml_diff>
--- a/market/MyStocks.xlsx
+++ b/market/MyStocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\my-projects\Other\market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB95707-279B-4BAF-9751-8EC760666F70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66EF647-11BF-4D74-B59A-6988DEAC9FE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-24930" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,8 +365,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;KFF8C00CONFIDENTIAL &amp; RESTRICTED&amp;1#</oddHeader>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>